<commit_message>
poprawki w algorytmie, dodatkowe obliczenia w pomiarach ruchu, zmiana dokumentacji (częściowo skończone)
</commit_message>
<xml_diff>
--- a/załącznik 2 - pomiary ruchu/pomiary 2.04.2016.xlsx
+++ b/załącznik 2 - pomiary ruchu/pomiary 2.04.2016.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>numer wlotu</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Pomiary zostały przeprowadzone 2 kwietnia 2016 roku w godzinach 14:30 - 15:30</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
   </si>
 </sst>
 </file>
@@ -57,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -160,11 +163,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -198,6 +214,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2666,11 +2690,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="183474048"/>
-        <c:axId val="183475584"/>
+        <c:axId val="91461504"/>
+        <c:axId val="91463040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="183474048"/>
+        <c:axId val="91461504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2682,12 +2706,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183475584"/>
+        <c:crossAx val="91463040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183475584"/>
+        <c:axId val="91463040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,7 +2722,137 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183474048"/>
+        <c:crossAx val="91461504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AH$3:$AH$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.97509569232738857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.403997576708135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6473450106294052</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7008128608004893</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7889102321918067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0837429692514413</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2152711957203164</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3180292455733666</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1014150125439417</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4783183622694458</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="104141568"/>
+        <c:axId val="104123008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="104141568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="104123008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="104123008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="104141568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2742,6 +2896,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3037,21 +3221,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+      <selection activeCell="AH3" sqref="AH3:AH13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" customWidth="1"/>
-    <col min="3" max="32" width="5.77734375" customWidth="1"/>
-    <col min="33" max="33" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+    <col min="3" max="32" width="5.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -3149,8 +3334,12 @@
       <c r="AG1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="AH1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI1" s="13"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3246,8 +3435,10 @@
         <v>1</v>
       </c>
       <c r="AG2" s="3"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="13"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3345,11 +3536,16 @@
         <v>5.6</v>
       </c>
       <c r="AG3" s="2">
-        <f>AVERAGE(C3:AF3)</f>
+        <f>AVERAGE($C3:$AF3)</f>
         <v>5.5543333333333313</v>
       </c>
+      <c r="AH3" s="15">
+        <f>STDEV($C3:$AF3)</f>
+        <v>0.97509569232738857</v>
+      </c>
+      <c r="AI3" s="16"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>2</v>
@@ -3445,11 +3641,16 @@
         <v>9.1</v>
       </c>
       <c r="AG4" s="2">
-        <f t="shared" ref="AG4:AG13" si="0">AVERAGE(C4:AF4)</f>
+        <f t="shared" ref="AG4:AG13" si="0">AVERAGE($C4:$AF4)</f>
         <v>8.1233333333333331</v>
       </c>
+      <c r="AH4" s="15">
+        <f t="shared" ref="AH4:AH13" si="1">STDEV($C4:$AF4)</f>
+        <v>1.403997576708135</v>
+      </c>
+      <c r="AI4" s="16"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1">
         <v>3</v>
@@ -3542,8 +3743,13 @@
         <f t="shared" si="0"/>
         <v>10.119259259259259</v>
       </c>
+      <c r="AH5" s="15">
+        <f t="shared" si="1"/>
+        <v>1.6473450106294052</v>
+      </c>
+      <c r="AI5" s="16"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>4</v>
@@ -3636,8 +3842,13 @@
         <f t="shared" si="0"/>
         <v>12.215185185185188</v>
       </c>
+      <c r="AH6" s="15">
+        <f t="shared" si="1"/>
+        <v>1.7008128608004893</v>
+      </c>
+      <c r="AI6" s="16"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1">
         <v>5</v>
@@ -3724,8 +3935,13 @@
         <f t="shared" si="0"/>
         <v>14.392083333333334</v>
       </c>
+      <c r="AH7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.7889102321918067</v>
+      </c>
+      <c r="AI7" s="16"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1">
         <v>6</v>
@@ -3806,8 +4022,13 @@
         <f t="shared" si="0"/>
         <v>16.60047619047619</v>
       </c>
+      <c r="AH8" s="15">
+        <f t="shared" si="1"/>
+        <v>2.0837429692514413</v>
+      </c>
+      <c r="AI8" s="16"/>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>7</v>
@@ -3880,8 +4101,13 @@
         <f t="shared" si="0"/>
         <v>18.754705882352944</v>
       </c>
+      <c r="AH9" s="15">
+        <f t="shared" si="1"/>
+        <v>2.2152711957203164</v>
+      </c>
+      <c r="AI9" s="16"/>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>8</v>
@@ -3952,8 +4178,13 @@
         <f t="shared" si="0"/>
         <v>21.019374999999997</v>
       </c>
+      <c r="AH10" s="15">
+        <f t="shared" si="1"/>
+        <v>2.3180292455733666</v>
+      </c>
+      <c r="AI10" s="16"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1">
         <v>9</v>
@@ -4020,8 +4251,13 @@
         <f t="shared" si="0"/>
         <v>23.042857142857144</v>
       </c>
+      <c r="AH11" s="15">
+        <f t="shared" si="1"/>
+        <v>2.1014150125439417</v>
+      </c>
+      <c r="AI11" s="16"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>10</v>
@@ -4071,11 +4307,16 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="2">
-        <f>AVERAGE(C12:AF12)</f>
+        <f t="shared" si="0"/>
         <v>24.855714285714281</v>
       </c>
+      <c r="AH12" s="15">
+        <f t="shared" si="1"/>
+        <v>2.4783183622694458</v>
+      </c>
+      <c r="AI12" s="16"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1">
         <v>11</v>
@@ -4120,8 +4361,13 @@
         <f t="shared" si="0"/>
         <v>24.716666666666669</v>
       </c>
+      <c r="AH13" s="15">
+        <f t="shared" si="1"/>
+        <v>0.88081401744825438</v>
+      </c>
+      <c r="AI13" s="16"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="U16" s="4" t="s">
         <v>4</v>
       </c>
@@ -4134,7 +4380,7 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="6"/>
     </row>
-    <row r="17" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U17" s="7"/>
       <c r="V17" s="8"/>
       <c r="W17" s="8"/>
@@ -4145,7 +4391,7 @@
       <c r="AB17" s="8"/>
       <c r="AC17" s="9"/>
     </row>
-    <row r="18" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U18" s="7"/>
       <c r="V18" s="8"/>
       <c r="W18" s="8"/>
@@ -4156,7 +4402,7 @@
       <c r="AB18" s="8"/>
       <c r="AC18" s="9"/>
     </row>
-    <row r="19" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U19" s="7"/>
       <c r="V19" s="8"/>
       <c r="W19" s="8"/>
@@ -4167,7 +4413,7 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="9"/>
     </row>
-    <row r="20" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U20" s="7"/>
       <c r="V20" s="8"/>
       <c r="W20" s="8"/>
@@ -4178,7 +4424,7 @@
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
     </row>
-    <row r="21" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U21" s="7"/>
       <c r="V21" s="8"/>
       <c r="W21" s="8"/>
@@ -4189,7 +4435,7 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="9"/>
     </row>
-    <row r="22" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U22" s="7"/>
       <c r="V22" s="8"/>
       <c r="W22" s="8"/>
@@ -4200,7 +4446,7 @@
       <c r="AB22" s="8"/>
       <c r="AC22" s="9"/>
     </row>
-    <row r="23" spans="21:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="21:29" x14ac:dyDescent="0.25">
       <c r="U23" s="10"/>
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
@@ -4212,11 +4458,13 @@
       <c r="AC23" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="U16:AC23"/>
     <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="AH1:AH2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4229,7 +4477,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4241,7 +4489,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dopisany rozdział 'zalącznik 1' w dokumentacji
</commit_message>
<xml_diff>
--- a/załącznik 2 - pomiary ruchu/pomiary 2.04.2016.xlsx
+++ b/załącznik 2 - pomiary ruchu/pomiary 2.04.2016.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>numer wlotu</t>
   </si>
@@ -27,13 +27,19 @@
     <t>numer pomiaru</t>
   </si>
   <si>
-    <t>average</t>
-  </si>
-  <si>
     <t>Pomiary zostały przeprowadzone 2 kwietnia 2016 roku w godzinach 14:30 - 15:30</t>
   </si>
   <si>
-    <t>standard deviation</t>
+    <t>średnia</t>
+  </si>
+  <si>
+    <t>odchylenie standardowe</t>
+  </si>
+  <si>
+    <t>numer samochodu</t>
+  </si>
+  <si>
+    <t>odch. st.</t>
   </si>
 </sst>
 </file>
@@ -180,10 +186,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -214,14 +225,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2690,11 +2707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91461504"/>
-        <c:axId val="91463040"/>
+        <c:axId val="92182400"/>
+        <c:axId val="92183936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91461504"/>
+        <c:axId val="92182400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2706,12 +2723,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91463040"/>
+        <c:crossAx val="92183936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91463040"/>
+        <c:axId val="92183936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2722,7 +2739,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91461504"/>
+        <c:crossAx val="92182400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2823,11 +2840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="104141568"/>
-        <c:axId val="104123008"/>
+        <c:axId val="91594112"/>
+        <c:axId val="92611712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104141568"/>
+        <c:axId val="91594112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,12 +2853,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104123008"/>
+        <c:crossAx val="92611712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104123008"/>
+        <c:axId val="92611712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2852,7 +2869,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104141568"/>
+        <c:crossAx val="91594112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2873,16 +2890,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>224118</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>233643</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>139065</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2903,16 +2920,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3221,10 +3238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI23"/>
+  <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AH13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3233,14 +3250,15 @@
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="32" width="5.7109375" customWidth="1"/>
     <col min="33" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.28515625" customWidth="1"/>
     <col min="35" max="35" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="1">
         <v>1</v>
       </c>
@@ -3331,19 +3349,19 @@
       <c r="AF1" s="1">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AG1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AI1" s="13"/>
+      <c r="AI1" s="5"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="1">
         <v>1</v>
       </c>
@@ -3434,9 +3452,9 @@
       <c r="AF2" s="1">
         <v>1</v>
       </c>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="13"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="5"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3539,11 +3557,11 @@
         <f>AVERAGE($C3:$AF3)</f>
         <v>5.5543333333333313</v>
       </c>
-      <c r="AH3" s="15">
+      <c r="AH3" s="3">
         <f>STDEV($C3:$AF3)</f>
         <v>0.97509569232738857</v>
       </c>
-      <c r="AI3" s="16"/>
+      <c r="AI3" s="4"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -3644,11 +3662,11 @@
         <f t="shared" ref="AG4:AG13" si="0">AVERAGE($C4:$AF4)</f>
         <v>8.1233333333333331</v>
       </c>
-      <c r="AH4" s="15">
+      <c r="AH4" s="3">
         <f t="shared" ref="AH4:AH13" si="1">STDEV($C4:$AF4)</f>
         <v>1.403997576708135</v>
       </c>
-      <c r="AI4" s="16"/>
+      <c r="AI4" s="4"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3743,11 +3761,11 @@
         <f t="shared" si="0"/>
         <v>10.119259259259259</v>
       </c>
-      <c r="AH5" s="15">
+      <c r="AH5" s="3">
         <f t="shared" si="1"/>
         <v>1.6473450106294052</v>
       </c>
-      <c r="AI5" s="16"/>
+      <c r="AI5" s="4"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -3842,11 +3860,11 @@
         <f t="shared" si="0"/>
         <v>12.215185185185188</v>
       </c>
-      <c r="AH6" s="15">
+      <c r="AH6" s="3">
         <f t="shared" si="1"/>
         <v>1.7008128608004893</v>
       </c>
-      <c r="AI6" s="16"/>
+      <c r="AI6" s="4"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -3935,11 +3953,11 @@
         <f t="shared" si="0"/>
         <v>14.392083333333334</v>
       </c>
-      <c r="AH7" s="15">
+      <c r="AH7" s="3">
         <f t="shared" si="1"/>
         <v>1.7889102321918067</v>
       </c>
-      <c r="AI7" s="16"/>
+      <c r="AI7" s="4"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -4022,11 +4040,11 @@
         <f t="shared" si="0"/>
         <v>16.60047619047619</v>
       </c>
-      <c r="AH8" s="15">
+      <c r="AH8" s="3">
         <f t="shared" si="1"/>
         <v>2.0837429692514413</v>
       </c>
-      <c r="AI8" s="16"/>
+      <c r="AI8" s="4"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -4101,11 +4119,11 @@
         <f t="shared" si="0"/>
         <v>18.754705882352944</v>
       </c>
-      <c r="AH9" s="15">
+      <c r="AH9" s="3">
         <f t="shared" si="1"/>
         <v>2.2152711957203164</v>
       </c>
-      <c r="AI9" s="16"/>
+      <c r="AI9" s="4"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -4178,11 +4196,11 @@
         <f t="shared" si="0"/>
         <v>21.019374999999997</v>
       </c>
-      <c r="AH10" s="15">
+      <c r="AH10" s="3">
         <f t="shared" si="1"/>
         <v>2.3180292455733666</v>
       </c>
-      <c r="AI10" s="16"/>
+      <c r="AI10" s="4"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -4251,11 +4269,11 @@
         <f t="shared" si="0"/>
         <v>23.042857142857144</v>
       </c>
-      <c r="AH11" s="15">
+      <c r="AH11" s="3">
         <f t="shared" si="1"/>
         <v>2.1014150125439417</v>
       </c>
-      <c r="AI11" s="16"/>
+      <c r="AI11" s="4"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -4310,11 +4328,11 @@
         <f t="shared" si="0"/>
         <v>24.855714285714281</v>
       </c>
-      <c r="AH12" s="15">
+      <c r="AH12" s="3">
         <f t="shared" si="1"/>
         <v>2.4783183622694458</v>
       </c>
-      <c r="AI12" s="16"/>
+      <c r="AI12" s="4"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -4361,104 +4379,1241 @@
         <f t="shared" si="0"/>
         <v>24.716666666666669</v>
       </c>
-      <c r="AH13" s="15">
+      <c r="AH13" s="3">
         <f t="shared" si="1"/>
         <v>0.88081401744825438</v>
       </c>
-      <c r="AI13" s="16"/>
+      <c r="AI13" s="4"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="U16" s="4" t="s">
+      <c r="U16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="9"/>
+    </row>
+    <row r="17" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F17" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="19"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="12"/>
+    </row>
+    <row r="18" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18" s="1">
         <v>4</v>
       </c>
-      <c r="V16" s="5"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="6"/>
+      <c r="L18" s="1">
+        <v>5</v>
+      </c>
+      <c r="M18" s="1">
+        <v>6</v>
+      </c>
+      <c r="N18" s="1">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1">
+        <v>8</v>
+      </c>
+      <c r="P18" s="1">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>10</v>
+      </c>
+      <c r="R18" s="4"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="12"/>
     </row>
-    <row r="17" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U17" s="7"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="9"/>
+    <row r="19" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>6.05</v>
+      </c>
+      <c r="I19" s="1">
+        <v>7.91</v>
+      </c>
+      <c r="J19" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="K19" s="1">
+        <v>12.02</v>
+      </c>
+      <c r="L19" s="1">
+        <v>13.98</v>
+      </c>
+      <c r="M19" s="1">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="4"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="12"/>
     </row>
-    <row r="18" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U18" s="7"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-      <c r="AA18" s="8"/>
-      <c r="AB18" s="8"/>
-      <c r="AC18" s="9"/>
+    <row r="20" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="I20" s="1">
+        <v>8.75</v>
+      </c>
+      <c r="J20" s="1">
+        <v>10.39</v>
+      </c>
+      <c r="K20" s="1">
+        <v>14.52</v>
+      </c>
+      <c r="L20" s="1">
+        <v>16.02</v>
+      </c>
+      <c r="M20" s="1">
+        <v>18.07</v>
+      </c>
+      <c r="N20" s="1">
+        <v>19.72</v>
+      </c>
+      <c r="O20" s="1">
+        <v>24.24</v>
+      </c>
+      <c r="P20" s="1">
+        <v>25.56</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>28.09</v>
+      </c>
+      <c r="R20" s="4"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="12"/>
     </row>
-    <row r="19" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U19" s="7"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-      <c r="AA19" s="8"/>
-      <c r="AB19" s="8"/>
-      <c r="AC19" s="9"/>
+    <row r="21" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1">
+        <v>5.86</v>
+      </c>
+      <c r="I21" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="J21" s="1">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="K21" s="1">
+        <v>10.92</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="4"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="12"/>
     </row>
-    <row r="20" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U20" s="7"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="8"/>
-      <c r="AA20" s="8"/>
-      <c r="AB20" s="8"/>
-      <c r="AC20" s="9"/>
+    <row r="22" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <v>4</v>
+      </c>
+      <c r="G22" s="1">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I22" s="1">
+        <v>6.27</v>
+      </c>
+      <c r="J22" s="1">
+        <v>8.32</v>
+      </c>
+      <c r="K22" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="L22" s="1">
+        <v>12.18</v>
+      </c>
+      <c r="M22" s="1">
+        <v>14.59</v>
+      </c>
+      <c r="N22" s="1">
+        <v>15.88</v>
+      </c>
+      <c r="O22" s="1">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="P22" s="1">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>21.2</v>
+      </c>
+      <c r="R22" s="4"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="12"/>
     </row>
-    <row r="21" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U21" s="7"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="8"/>
-      <c r="AA21" s="8"/>
-      <c r="AB21" s="8"/>
-      <c r="AC21" s="9"/>
+    <row r="23" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <v>5</v>
+      </c>
+      <c r="G23" s="1">
+        <v>7</v>
+      </c>
+      <c r="H23" s="1">
+        <v>5.41</v>
+      </c>
+      <c r="I23" s="1">
+        <v>7.25</v>
+      </c>
+      <c r="J23" s="1">
+        <v>8.66</v>
+      </c>
+      <c r="K23" s="1">
+        <v>10.42</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="4"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="15"/>
     </row>
-    <row r="22" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U22" s="7"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
-      <c r="Z22" s="8"/>
-      <c r="AA22" s="8"/>
-      <c r="AB22" s="8"/>
-      <c r="AC22" s="9"/>
+    <row r="24" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>8</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3.77</v>
+      </c>
+      <c r="I24" s="1">
+        <v>5.27</v>
+      </c>
+      <c r="J24" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="K24" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="L24" s="1">
+        <v>11.03</v>
+      </c>
+      <c r="M24" s="1">
+        <v>13.09</v>
+      </c>
+      <c r="N24" s="1">
+        <v>15.83</v>
+      </c>
+      <c r="O24" s="1">
+        <v>21.54</v>
+      </c>
+      <c r="P24" s="1">
+        <v>25.83</v>
+      </c>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="4"/>
     </row>
-    <row r="23" spans="21:29" x14ac:dyDescent="0.25">
-      <c r="U23" s="10"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
-      <c r="AC23" s="12"/>
+    <row r="25" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F25" s="1">
+        <v>7</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="I25" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="J25" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K25" s="1">
+        <v>12.46</v>
+      </c>
+      <c r="L25" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="M25" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="N25" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="O25" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F26" s="1">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3</v>
+      </c>
+      <c r="H26" s="1">
+        <v>4.08</v>
+      </c>
+      <c r="I26" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="J26" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="K26" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="L26" s="1">
+        <v>12</v>
+      </c>
+      <c r="M26" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="4"/>
+    </row>
+    <row r="27" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F27" s="1">
+        <v>9</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I27" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="J27" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="K27" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>13.7</v>
+      </c>
+      <c r="M27" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="N27" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="O27" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="P27" s="1">
+        <v>21.7</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>24</v>
+      </c>
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F28" s="1">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1">
+        <v>9</v>
+      </c>
+      <c r="H28" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="I28" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J28" s="1">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1">
+        <v>13.7</v>
+      </c>
+      <c r="L28" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="M28" s="1">
+        <v>18</v>
+      </c>
+      <c r="N28" s="1">
+        <v>20</v>
+      </c>
+      <c r="O28" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="P28" s="1">
+        <v>24</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>26</v>
+      </c>
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F29" s="1">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1">
+        <v>7</v>
+      </c>
+      <c r="H29" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="I29" s="1">
+        <v>9</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F30" s="1">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1">
+        <v>8</v>
+      </c>
+      <c r="H30" s="1">
+        <v>6.01</v>
+      </c>
+      <c r="I30" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="J30" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="K30" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="L30" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="M30" s="1">
+        <v>14.41</v>
+      </c>
+      <c r="N30" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="O30" s="1">
+        <v>17.39</v>
+      </c>
+      <c r="P30" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="4"/>
+    </row>
+    <row r="31" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F31" s="1">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I31" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="J31" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K31" s="1">
+        <v>11</v>
+      </c>
+      <c r="L31" s="1">
+        <v>15</v>
+      </c>
+      <c r="M31" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="N31" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="O31" s="1">
+        <v>23.4</v>
+      </c>
+      <c r="P31" s="1">
+        <v>24.9</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>27.6</v>
+      </c>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="6:29" x14ac:dyDescent="0.25">
+      <c r="F32" s="1">
+        <v>14</v>
+      </c>
+      <c r="G32" s="1">
+        <v>9</v>
+      </c>
+      <c r="H32" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="I32" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="J32" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="K32" s="1">
+        <v>14</v>
+      </c>
+      <c r="L32" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="M32" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="N32" s="1">
+        <v>23.1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>25.1</v>
+      </c>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="4"/>
+    </row>
+    <row r="33" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F33" s="1">
+        <v>15</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4</v>
+      </c>
+      <c r="H33" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="I33" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="4"/>
+    </row>
+    <row r="34" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F34" s="1">
+        <v>16</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I34" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="J34" s="1">
+        <v>10</v>
+      </c>
+      <c r="K34" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="L34" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="M34" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="N34" s="1">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="O34" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="P34" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>23.4</v>
+      </c>
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <v>17</v>
+      </c>
+      <c r="G35" s="1">
+        <v>8</v>
+      </c>
+      <c r="H35" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I35" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="J35" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="K35" s="1">
+        <v>11</v>
+      </c>
+      <c r="L35" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="M35" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="N35" s="1">
+        <v>18</v>
+      </c>
+      <c r="O35" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="P35" s="1">
+        <v>21.77</v>
+      </c>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="4"/>
+    </row>
+    <row r="36" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F36" s="1">
+        <v>18</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
+      </c>
+      <c r="H36" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="I36" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="J36" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="K36" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="L36" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="4"/>
+    </row>
+    <row r="37" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F37" s="1">
+        <v>19</v>
+      </c>
+      <c r="G37" s="1">
+        <v>3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="I37" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J37" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="K37" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="L37" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="M37" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="4"/>
+    </row>
+    <row r="38" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F38" s="1">
+        <v>20</v>
+      </c>
+      <c r="G38" s="1">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J38" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="K38" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="L38" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="4"/>
+    </row>
+    <row r="39" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F39" s="1">
+        <v>21</v>
+      </c>
+      <c r="G39" s="1">
+        <v>8</v>
+      </c>
+      <c r="H39" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="I39" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="J39" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K39" s="1">
+        <v>12</v>
+      </c>
+      <c r="L39" s="1">
+        <v>14.4</v>
+      </c>
+      <c r="M39" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="N39" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="O39" s="1">
+        <v>21.9</v>
+      </c>
+      <c r="P39" s="1">
+        <v>25.3</v>
+      </c>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="4"/>
+    </row>
+    <row r="40" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F40" s="1">
+        <v>22</v>
+      </c>
+      <c r="G40" s="1">
+        <v>9</v>
+      </c>
+      <c r="H40" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I40" s="1">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="K40" s="1">
+        <v>13.8</v>
+      </c>
+      <c r="L40" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="M40" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="N40" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="O40" s="1">
+        <v>21.1</v>
+      </c>
+      <c r="P40" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="4"/>
+    </row>
+    <row r="41" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F41" s="1">
+        <v>23</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3</v>
+      </c>
+      <c r="H41" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="J41" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="K41" s="1">
+        <v>14</v>
+      </c>
+      <c r="L41" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="4"/>
+    </row>
+    <row r="42" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F42" s="1">
+        <v>24</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1</v>
+      </c>
+      <c r="H42" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="I42" s="1">
+        <v>7</v>
+      </c>
+      <c r="J42" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K42" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="L42" s="1">
+        <v>13</v>
+      </c>
+      <c r="M42" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="N42" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="O42" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="P42" s="1">
+        <v>20.3</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>23.7</v>
+      </c>
+      <c r="R42" s="4"/>
+    </row>
+    <row r="43" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F43" s="1">
+        <v>25</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="I43" s="1">
+        <v>8</v>
+      </c>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="4"/>
+    </row>
+    <row r="44" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F44" s="1">
+        <v>26</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="I44" s="1">
+        <v>8</v>
+      </c>
+      <c r="J44" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K44" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="4"/>
+    </row>
+    <row r="45" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <v>27</v>
+      </c>
+      <c r="G45" s="1">
+        <v>8</v>
+      </c>
+      <c r="H45" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I45" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="J45" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="K45" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="L45" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="M45" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="4"/>
+    </row>
+    <row r="46" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
+        <v>28</v>
+      </c>
+      <c r="G46" s="1">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="I46" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="J46" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="K46" s="1">
+        <v>13.8</v>
+      </c>
+      <c r="L46" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="M46" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="N46" s="1">
+        <v>21.1</v>
+      </c>
+      <c r="O46" s="1">
+        <v>22</v>
+      </c>
+      <c r="P46" s="1">
+        <v>23.3</v>
+      </c>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="4"/>
+    </row>
+    <row r="47" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
+        <v>29</v>
+      </c>
+      <c r="G47" s="1">
+        <v>3</v>
+      </c>
+      <c r="H47" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="I47" s="1">
+        <v>10</v>
+      </c>
+      <c r="J47" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="K47" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="L47" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="M47" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="N47" s="1">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="4"/>
+    </row>
+    <row r="48" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F48" s="1">
+        <v>30</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1</v>
+      </c>
+      <c r="H48" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="I48" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="J48" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="K48" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="L48" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="M48" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="N48" s="1">
+        <v>21.9</v>
+      </c>
+      <c r="O48" s="1">
+        <v>23.4</v>
+      </c>
+      <c r="P48" s="1">
+        <v>24.6</v>
+      </c>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="4"/>
+    </row>
+    <row r="49" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="2">
+        <f>AVERAGE(H$19:H$48)</f>
+        <v>5.5543333333333313</v>
+      </c>
+      <c r="I49" s="2">
+        <f>AVERAGE(I$19:I$48)</f>
+        <v>8.1233333333333331</v>
+      </c>
+      <c r="J49" s="2">
+        <f>AVERAGE(J$19:J$48)</f>
+        <v>10.119259259259259</v>
+      </c>
+      <c r="K49" s="2">
+        <f>AVERAGE(K$19:K$48)</f>
+        <v>12.215185185185188</v>
+      </c>
+      <c r="L49" s="2">
+        <f>AVERAGE(L$19:L$48)</f>
+        <v>14.392083333333334</v>
+      </c>
+      <c r="M49" s="2">
+        <f>AVERAGE(M$19:M$48)</f>
+        <v>16.60047619047619</v>
+      </c>
+      <c r="N49" s="2">
+        <f>AVERAGE(N$19:N$48)</f>
+        <v>18.754705882352944</v>
+      </c>
+      <c r="O49" s="2">
+        <f>AVERAGE(O$19:O$48)</f>
+        <v>21.019374999999997</v>
+      </c>
+      <c r="P49" s="2">
+        <f>AVERAGE(P$19:P$48)</f>
+        <v>23.042857142857144</v>
+      </c>
+      <c r="Q49" s="18">
+        <f>AVERAGE(Q$19:Q$48)</f>
+        <v>24.855714285714281</v>
+      </c>
+      <c r="R49" s="20"/>
+    </row>
+    <row r="50" spans="6:18" x14ac:dyDescent="0.25">
+      <c r="F50" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="3">
+        <f>STDEV(H$19:H$48)</f>
+        <v>0.97509569232738857</v>
+      </c>
+      <c r="I50" s="3">
+        <f>STDEV(I$19:I$48)</f>
+        <v>1.403997576708135</v>
+      </c>
+      <c r="J50" s="3">
+        <f>STDEV(J$19:J$48)</f>
+        <v>1.6473450106294052</v>
+      </c>
+      <c r="K50" s="3">
+        <f>STDEV(K$19:K$48)</f>
+        <v>1.7008128608004893</v>
+      </c>
+      <c r="L50" s="3">
+        <f>STDEV(L$19:L$48)</f>
+        <v>1.7889102321918067</v>
+      </c>
+      <c r="M50" s="3">
+        <f>STDEV(M$19:M$48)</f>
+        <v>2.0837429692514413</v>
+      </c>
+      <c r="N50" s="3">
+        <f>STDEV(N$19:N$48)</f>
+        <v>2.2152711957203164</v>
+      </c>
+      <c r="O50" s="3">
+        <f>STDEV(O$19:O$48)</f>
+        <v>2.3180292455733666</v>
+      </c>
+      <c r="P50" s="3">
+        <f>STDEV(P$19:P$48)</f>
+        <v>2.1014150125439417</v>
+      </c>
+      <c r="Q50" s="3">
+        <f>STDEV(Q$19:Q$48)</f>
+        <v>2.4783183622694458</v>
+      </c>
+      <c r="R50" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:Q17"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>